<commit_message>
add randomTimes for  index page
</commit_message>
<xml_diff>
--- a/excel/Excel_BTS_Portfolio (version 1).xlsx
+++ b/excel/Excel_BTS_Portfolio (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugo\OneDrive\Bureau\PERSO\PORTFOLIO\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6577AF2A-EF9D-49B3-993B-74ED08126E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373BC9AF-F731-4469-B7B0-2977C7DE2422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$35</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -49,9 +48,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
-  </si>
-  <si>
-    <t xml:space="preserve">N° candidat : </t>
   </si>
   <si>
     <t>Centre de formation : EPSI Lille</t>
@@ -128,9 +124,6 @@
 </t>
   </si>
   <si>
-    <t>Dec 22</t>
-  </si>
-  <si>
     <t>Commande Base de données SQL</t>
   </si>
   <si>
@@ -146,9 +139,6 @@
     <t>NOM et prénom : Hochart Hugo</t>
   </si>
   <si>
-    <t>Adresse URL du portfolio : hochart.heb3.org</t>
-  </si>
-  <si>
     <t>Réalisation de gestionnaire de stock en HTML/CSS/PhpMyAdmin</t>
   </si>
   <si>
@@ -209,9 +199,6 @@
     <t xml:space="preserve">Création d'un site e-commerce de vente de chaussure en React </t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Application de stock</t>
   </si>
   <si>
@@ -219,6 +206,75 @@
   </si>
   <si>
     <t>Réalisations en milieu professionnel en cours de deuxième année</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://hugo-hochart.web-edu.fr/</t>
+  </si>
+  <si>
+    <t>N° candidat :  02047327769</t>
+  </si>
+  <si>
+    <t>22/11/22 au 08/12/22</t>
+  </si>
+  <si>
+    <t>16/01/23 au 17/01/23</t>
+  </si>
+  <si>
+    <t>20/02/23 au 26/04/23</t>
+  </si>
+  <si>
+    <t>20/02/23 au 21/02/23</t>
+  </si>
+  <si>
+    <t>09/02/23 au 23/02/23</t>
+  </si>
+  <si>
+    <t>20/03/23 au 26/06/23</t>
+  </si>
+  <si>
+    <t>25/09/23 au 25/10/23</t>
+  </si>
+  <si>
+    <t>10/12/23 au 25/04/24</t>
+  </si>
+  <si>
+    <t>02/12/23 au 18/12/23</t>
+  </si>
+  <si>
+    <t>03/11/23 au 15/11/23</t>
+  </si>
+  <si>
+    <t>05/12/23 au 20/03/24</t>
+  </si>
+  <si>
+    <t>18/03/24 au 09/04/24</t>
+  </si>
+  <si>
+    <t>24/02/24 au 08/03/24</t>
+  </si>
+  <si>
+    <t>03/03/24 au 27/04/24</t>
+  </si>
+  <si>
+    <t>10/11/23 au 22/12/23</t>
+  </si>
+  <si>
+    <t>20/03/23 au 10/04/23</t>
+  </si>
+  <si>
+    <t>16/01/23 au 20/01/23</t>
+  </si>
+  <si>
+    <t>10/11/22 au 16/01/23</t>
+  </si>
+  <si>
+    <t>20/02/23 au 07/03/23</t>
+  </si>
+  <si>
+    <t>15/05/2023 au 23/06/2023</t>
+  </si>
+  <si>
+    <t>02/01/2024 au 23/02/2024</t>
   </si>
 </sst>
 </file>
@@ -447,7 +503,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -524,9 +580,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -545,59 +598,67 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -910,136 +971,138 @@
   </sheetPr>
   <dimension ref="A1:AQ77"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScale="90" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" style="1" customWidth="1"/>
     <col min="3" max="8" width="18.6640625" style="1" customWidth="1"/>
-    <col min="9" max="43" width="10.88671875" customWidth="1"/>
+    <col min="9" max="12" width="10.88671875" customWidth="1"/>
+    <col min="13" max="13" width="20.77734375" customWidth="1"/>
+    <col min="14" max="43" width="10.88671875" customWidth="1"/>
     <col min="44" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="48"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:43" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="50"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="46"/>
     </row>
     <row r="3" spans="1:43" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="40"/>
+      <c r="A3" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="41"/>
+      <c r="H3" s="42"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="10" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="10" t="s">
-        <v>5</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="40"/>
+      <c r="A5" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="42"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="C6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="D6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="G6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="H6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="18" t="s">
+    </row>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="325.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="43"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="325.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="13" t="s">
+      <c r="D7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="E7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="G7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="H7" s="19" t="s">
         <v>18</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>19</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1078,16 +1141,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="38"/>
+      <c r="A8" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="36"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1130,7 +1193,7 @@
       <c r="C9" s="15"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="31"/>
+      <c r="F9" s="30"/>
       <c r="G9" s="4"/>
       <c r="H9" s="21"/>
       <c r="I9"/>
@@ -1170,18 +1233,18 @@
       <c r="AQ9"/>
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>21</v>
+      <c r="A10" s="50" t="s">
+        <v>20</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="42"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="33"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1219,18 +1282,18 @@
       <c r="AQ10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="14">
-        <v>44866</v>
+      <c r="A11" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="27"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="26"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1268,18 +1331,18 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="14">
-        <v>44927</v>
+      <c r="A12" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="42"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="33"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1317,18 +1380,18 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="9">
-        <v>44866</v>
-      </c>
-      <c r="C13" s="30"/>
+      <c r="A13" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="29"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
-      <c r="F13" s="31"/>
+      <c r="F13" s="30"/>
       <c r="G13" s="16"/>
-      <c r="H13" s="28"/>
+      <c r="H13" s="27"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1366,16 +1429,18 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="30"/>
+      <c r="A14" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="29"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="42"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="33"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1413,18 +1478,18 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="30" t="s">
-        <v>49</v>
-      </c>
+      <c r="A15" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="29"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="42"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="33"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1462,14 +1527,16 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="30"/>
+      <c r="A16" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="29"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="30"/>
+      <c r="F16" s="29"/>
       <c r="G16" s="4"/>
       <c r="H16" s="21"/>
       <c r="I16"/>
@@ -1509,16 +1576,18 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="3"/>
+      <c r="A17" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="49" t="s">
+        <v>66</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="29"/>
+      <c r="F17" s="28"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="42"/>
+      <c r="H17" s="33"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1556,16 +1625,18 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="3"/>
+      <c r="A18" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="49" t="s">
+        <v>55</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1603,16 +1674,18 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="30"/>
+      <c r="A19" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="29"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="42"/>
+      <c r="H19" s="33"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1650,18 +1723,18 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="30" t="s">
-        <v>49</v>
-      </c>
+      <c r="A20" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="29"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="42"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="33"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -1699,18 +1772,18 @@
       <c r="AQ20"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="30" t="s">
-        <v>49</v>
-      </c>
+      <c r="A21" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="29"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="42"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="33"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -1748,18 +1821,18 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="30" t="s">
-        <v>49</v>
-      </c>
+      <c r="A22" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="29"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="42"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="33"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -1797,16 +1870,18 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="3"/>
+      <c r="A23" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>59</v>
+      </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="32"/>
+      <c r="F23" s="31"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="42"/>
+      <c r="H23" s="33"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -1844,16 +1919,18 @@
       <c r="AQ23"/>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="30"/>
+      <c r="A24" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="29"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="42"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="33"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -1891,15 +1968,17 @@
       <c r="AQ24"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="3"/>
+      <c r="A25" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="49" t="s">
+        <v>60</v>
+      </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="3"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
       <c r="H25" s="23"/>
       <c r="I25"/>
       <c r="J25"/>
@@ -1938,18 +2017,18 @@
       <c r="AQ25"/>
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="30" t="s">
-        <v>49</v>
-      </c>
+      <c r="A26" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="29"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="42"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="33"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -1987,16 +2066,18 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="3"/>
+      <c r="A27" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="49" t="s">
+        <v>62</v>
+      </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="42"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="33"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2034,16 +2115,18 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="3"/>
+      <c r="A28" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>63</v>
+      </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="42"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="33"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2081,16 +2164,16 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A29" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="38"/>
+      <c r="A29" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="36"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2131,7 +2214,7 @@
       <c r="A30" s="22"/>
       <c r="B30" s="3"/>
       <c r="C30" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -2176,15 +2259,17 @@
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="41"/>
+        <v>26</v>
+      </c>
+      <c r="B31" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="32"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="42"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="33"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2223,15 +2308,17 @@
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="B32" s="49" t="s">
+        <v>70</v>
+      </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="30"/>
+      <c r="D32" s="29"/>
       <c r="E32" s="5"/>
       <c r="F32" s="3"/>
       <c r="G32" s="5"/>
-      <c r="H32" s="42"/>
+      <c r="H32" s="33"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2270,14 +2357,16 @@
     </row>
     <row r="33" spans="1:43" s="2" customFormat="1" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
+        <v>27</v>
+      </c>
+      <c r="B33" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="30"/>
+      <c r="G33" s="29"/>
       <c r="H33" s="23"/>
       <c r="I33"/>
       <c r="J33"/>
@@ -2361,16 +2450,16 @@
       <c r="AQ34"/>
     </row>
     <row r="35" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A35" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="38"/>
+      <c r="A35" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="36"/>
       <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>
@@ -2411,7 +2500,7 @@
       <c r="A36" s="22"/>
       <c r="B36" s="3"/>
       <c r="C36" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -2421,15 +2510,17 @@
     </row>
     <row r="37" spans="1:43" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="30"/>
+        <v>31</v>
+      </c>
+      <c r="B37" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="29"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="30"/>
+      <c r="E37" s="29"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="42"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="33"/>
     </row>
     <row r="38" spans="1:43" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A38" s="24"/>

</xml_diff>